<commit_message>
Adapt tests to control version
</commit_message>
<xml_diff>
--- a/formshare/tests/resources/forms/GeoJSON/GeoJSON.xlsx
+++ b/formshare/tests/resources/forms/GeoJSON/GeoJSON.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t xml:space="preserve">form_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version</t>
   </si>
   <si>
     <t xml:space="preserve">Just an example of GeoJSON</t>
@@ -350,7 +353,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.19"/>
@@ -502,7 +505,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.64"/>
@@ -595,13 +598,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.41"/>
@@ -615,13 +618,19 @@
       <c r="B1" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>